<commit_message>
Thêm danh sách chức vụ
</commit_message>
<xml_diff>
--- a/src/main/java/files/DSNamHoc.xlsx
+++ b/src/main/java/files/DSNamHoc.xlsx
@@ -6,33 +6,48 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DanhSachNamHoc" r:id="rId3" sheetId="1"/>
+    <sheet name="DanhSachChucVu" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t>Mã năm học</t>
+    <t>Mã chức vụ</t>
   </si>
   <si>
-    <t>Năm học</t>
+    <t>Tên chức vụ</t>
   </si>
   <si>
     <t>Trạng thái hiển thị</t>
   </si>
   <si>
-    <t>2022-2023</t>
+    <t>BCS</t>
   </si>
   <si>
-    <t>Ẩn</t>
-  </si>
-  <si>
-    <t>2023-2024</t>
+    <t>Ban cán sự</t>
   </si>
   <si>
     <t>Hiển thị</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cố vấn học tập </t>
+  </si>
+  <si>
+    <t>QL</t>
+  </si>
+  <si>
+    <t>Quản lý</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>Sinh viên</t>
   </si>
 </sst>
 </file>
@@ -77,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -95,25 +110,47 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
+      <c r="A2" t="s" s="0">
+        <v>3</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>2.0</v>
+      <c r="A3" t="s" s="0">
+        <v>6</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>6</v>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>